<commit_message>
New execution: Pressure Vessel.
New execution: Pressure Vessel.
</commit_message>
<xml_diff>
--- a/Results/Matlab/Matlab executions.xlsx
+++ b/Results/Matlab/Matlab executions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\Tesis Adrian\Article SoftwareX\JMetaBFOP_EN CORECCIÓN  2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\JMetaBFOP-UI\Results\Matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E695E427-C53D-4D39-8817-59B2E77C31AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A6E4B-543C-4337-8659-2BEC6AAC4A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="21" xr2:uid="{790385BC-1074-4F4F-916A-C4954E51DCAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{790385BC-1074-4F4F-916A-C4954E51DCAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tension-Compression S" sheetId="1" r:id="rId1"/>
@@ -1544,8 +1544,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1629,7 +1630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1653,7 +1654,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1981,7 +1988,7 @@
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1989,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>1.26750279823777E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2005,7 +2012,7 @@
         <v>1.26655384666384E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2013,7 +2020,7 @@
         <v>1.2672148339278501E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2021,7 +2028,7 @@
         <v>1.26732855390944E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>1.2665232788448499E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2049,7 +2056,7 @@
         <v>1.2665435486926099E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2062,9 +2069,8 @@
       <c r="F8">
         <v>1.2665239599783299E-2</v>
       </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2078,7 +2084,7 @@
         <v>3.3931763009982E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>1.2666416057541501E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2106,7 +2112,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2134,7 +2140,7 @@
         <v>2214.3000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2142,7 +2148,7 @@
         <v>1.26762062438607E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2150,7 +2156,7 @@
         <v>1.2667918128380499E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -6509,8 +6515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAC26F2-455B-4B7D-8607-0956394F0263}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6520,7 +6526,7 @@
     <col min="7" max="7" width="66.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6528,178 +6534,179 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>5958.6293929927497</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5885.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5885.3332510914697</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5885.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>5885.33282922129</v>
+        <v>5885.3</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="E4">
-        <v>5885.3327736973197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="12">
+        <v>5885.3328000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>5887.6905601832595</v>
+        <v>5885.3</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="E5">
-        <v>5910.2411576191698</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="12">
+        <v>5885.3</v>
+      </c>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>5953.8024491502401</v>
+        <v>5885.3</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6">
-        <v>5888.3143108902204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="13">
+        <v>5885.3371695695196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>5924.3655319279596</v>
+        <v>5885.3</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="12">
+        <v>1.2347787208473E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>5924.9486528431798</v>
+        <v>5885.3</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="E8">
-        <v>6061.1076314992297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="12">
+        <v>5885.4371695695199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>5942.0480473793896</v>
+        <v>5885.3</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5885.7632041414499</v>
+        <v>5885.3</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>5885.3740456714204</v>
+        <v>5885.3</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>5886.7164181040198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+        <v>5885.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>5885.4443154525197</v>
+        <v>5885.3</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>5888.9380615971704</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+        <v>5885.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>5901.84842977894</v>
+        <v>5885.3</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>5885.3327736973197</v>
+        <v>5885.3</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -6708,7 +6715,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>5894.8014875283998</v>
+        <v>5885.3</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>4</v>
@@ -6719,7 +6726,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>5945.02276348343</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -6727,7 +6734,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>5907.60867337731</v>
+        <v>5885.3</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>5</v>
@@ -6738,7 +6745,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>5885.9714864846701</v>
+        <v>5885.4</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="33" x14ac:dyDescent="0.25">
@@ -6746,7 +6753,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>5885.3427048038002</v>
+        <v>5885.3</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>10</v>
@@ -6757,7 +6764,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>5957.4821525357702</v>
+        <v>5885.3</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -6766,7 +6773,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>5885.3625667411097</v>
+        <v>5885.3</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>4</v>
@@ -6777,7 +6784,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>6048.7482055503096</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -6785,7 +6792,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>5907.7887224655997</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -6793,7 +6800,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>5947.8161711286502</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6801,7 +6808,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>5914.9268923091004</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -6809,7 +6816,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>5885.3643864468704</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -6817,7 +6824,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>5885.3328076285297</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -6825,7 +6832,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>5887.5912590143798</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -6833,7 +6840,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>5886.5064858449095</v>
+        <v>5885.3</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -7108,6 +7115,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7155,7 +7163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C078A562-5807-43CB-BF6D-5D4BABF7E7C0}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>